<commit_message>
Results for NTRANS konferanse
Inkludert VSS
</commit_message>
<xml_diff>
--- a/Data/scenarios.xlsx
+++ b/Data/scenarios.xlsx
@@ -5,19 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\egbertrv\Documents\GitHub\AIM_Norwegian_Freight_Model\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/steffejb_ntnu_no/Documents/Work/GitHub/AIM_Norwegian_Freight_Model/AIM_Norwegian_Freight_Model/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9C4C2C-16B4-4594-A85E-155303F6E56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{4D9C4C2C-16B4-4594-A85E-155303F6E56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA372F63-05CF-4CE1-AAA2-41A88672A5A1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13800" yWindow="0" windowWidth="30345" windowHeight="23400" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenarios_base" sheetId="1" r:id="rId1"/>
     <sheet name="three_scenarios" sheetId="4" r:id="rId2"/>
     <sheet name="three_scenarios_new" sheetId="5" r:id="rId3"/>
-    <sheet name="variability" sheetId="3" r:id="rId4"/>
-    <sheet name="fuel_groups" sheetId="2" r:id="rId5"/>
+    <sheet name="EV_scenario" sheetId="6" r:id="rId4"/>
+    <sheet name="variability" sheetId="3" r:id="rId5"/>
+    <sheet name="fuel_groups" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="65">
   <si>
     <t>Scenario</t>
   </si>
@@ -564,7 +565,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="A15" sqref="A15:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1828,7 +1829,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:N3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2005,6 +2006,91 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F34A01C7-0A25-459C-A739-C90077084666}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E8D1424-7946-4BE5-99E5-DF2D4339CAC6}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2030,7 +2116,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAD9A92-DA97-41D6-8F28-B69416D7D7DA}">
   <dimension ref="A1:C19"/>
   <sheetViews>

</xml_diff>

<commit_message>
Created setting with nine scenarios
</commit_message>
<xml_diff>
--- a/Data/scenarios.xlsx
+++ b/Data/scenarios.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\egbertrv\Documents\GitHub\AIM_Norwegian_Freight_Model\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79EE936-1B99-4011-8F1A-FA86D3C0BA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0055DE63-B91E-4D5A-836C-689BD6F502BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenarios_base" sheetId="1" r:id="rId1"/>
-    <sheet name="three_scenarios" sheetId="4" r:id="rId2"/>
-    <sheet name="three_scenarios_new" sheetId="5" r:id="rId3"/>
-    <sheet name="EV_scenario" sheetId="6" r:id="rId4"/>
-    <sheet name="variability" sheetId="3" r:id="rId5"/>
-    <sheet name="fuel_groups" sheetId="2" r:id="rId6"/>
+    <sheet name="nine_scenarios" sheetId="7" r:id="rId2"/>
+    <sheet name="three_scenarios" sheetId="4" r:id="rId3"/>
+    <sheet name="three_scenarios_new" sheetId="5" r:id="rId4"/>
+    <sheet name="EV_scenario" sheetId="6" r:id="rId5"/>
+    <sheet name="variability" sheetId="3" r:id="rId6"/>
+    <sheet name="fuel_groups" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="66">
   <si>
     <t>Scenario</t>
   </si>
@@ -568,7 +569,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection sqref="A1:K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1652,6 +1653,405 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D8424FF-558A-4FF4-BD92-4595B5988325}">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <f>1/9</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C10" si="0">1/9</f>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f>1-variability!$A$2</f>
+        <v>0.75</v>
+      </c>
+      <c r="F3">
+        <f>1-variability!$A$2</f>
+        <v>0.75</v>
+      </c>
+      <c r="G3">
+        <f>1-variability!$A$2</f>
+        <v>0.75</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f>1-variability!$A$2</f>
+        <v>0.75</v>
+      </c>
+      <c r="F4">
+        <f>1-variability!$A$2</f>
+        <v>0.75</v>
+      </c>
+      <c r="G4">
+        <f>1+variability!$A$2</f>
+        <v>1.25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <f>1-variability!$A$2</f>
+        <v>0.75</v>
+      </c>
+      <c r="F5">
+        <f>1+variability!$A$2</f>
+        <v>1.25</v>
+      </c>
+      <c r="G5">
+        <f>1-variability!$A$2</f>
+        <v>0.75</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <f>1-variability!$A$2</f>
+        <v>0.75</v>
+      </c>
+      <c r="F6">
+        <f>1+variability!$A$2</f>
+        <v>1.25</v>
+      </c>
+      <c r="G6">
+        <f>1+variability!$A$2</f>
+        <v>1.25</v>
+      </c>
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <f>1+variability!$A$2</f>
+        <v>1.25</v>
+      </c>
+      <c r="F7">
+        <f>1-variability!$A$2</f>
+        <v>0.75</v>
+      </c>
+      <c r="G7">
+        <f>1-variability!$A$2</f>
+        <v>0.75</v>
+      </c>
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <f>1+variability!$A$2</f>
+        <v>1.25</v>
+      </c>
+      <c r="F8">
+        <f>1-variability!$A$2</f>
+        <v>0.75</v>
+      </c>
+      <c r="G8">
+        <f>1+variability!$A$2</f>
+        <v>1.25</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <f>1+variability!$A$2</f>
+        <v>1.25</v>
+      </c>
+      <c r="F9">
+        <f>1+variability!$A$2</f>
+        <v>1.25</v>
+      </c>
+      <c r="G9">
+        <f>1-variability!$A$2</f>
+        <v>0.75</v>
+      </c>
+      <c r="H9" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" t="s">
+        <v>36</v>
+      </c>
+      <c r="J9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f>1+variability!$A$2</f>
+        <v>1.25</v>
+      </c>
+      <c r="F10">
+        <f>1+variability!$A$2</f>
+        <v>1.25</v>
+      </c>
+      <c r="G10">
+        <f>1+variability!$A$2</f>
+        <v>1.25</v>
+      </c>
+      <c r="H10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59180BE-5606-40D4-8893-B1262E6F265B}">
   <dimension ref="A1:K4"/>
   <sheetViews>
@@ -1827,7 +2227,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BC66704-B169-4E35-BB26-DD18B5F91B22}">
   <dimension ref="A1:M5"/>
   <sheetViews>
@@ -2047,12 +2447,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F34A01C7-0A25-459C-A739-C90077084666}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2133,7 +2533,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E8D1424-7946-4BE5-99E5-DF2D4339CAC6}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -2159,7 +2559,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAD9A92-DA97-41D6-8F28-B69416D7D7DA}">
   <dimension ref="A1:C19"/>
   <sheetViews>

</xml_diff>

<commit_message>
merging Steffen and Ruben
</commit_message>
<xml_diff>
--- a/Data/scenarios.xlsx
+++ b/Data/scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\home.ansatt.ntnu.no\egbertrv\Documents\GitHub\AIM_Norwegian_Freight_Model\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\STraM_ntnu_development\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0055DE63-B91E-4D5A-836C-689BD6F502BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B91EB177-2576-411F-894F-3F98FD906274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenarios_base" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="three_scenarios_new" sheetId="5" r:id="rId4"/>
     <sheet name="EV_scenario" sheetId="6" r:id="rId5"/>
     <sheet name="variability" sheetId="3" r:id="rId6"/>
-    <sheet name="fuel_groups" sheetId="2" r:id="rId7"/>
+    <sheet name="fuel_groups (backup)" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="65">
   <si>
     <t>Scenario</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>Battery</t>
-  </si>
-  <si>
-    <t>Biofuel</t>
   </si>
   <si>
     <t>Probability</t>
@@ -569,7 +566,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K28"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,34 +587,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -625,7 +622,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <f>1/27</f>
@@ -647,16 +644,16 @@
         <v>0.75</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -664,7 +661,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C28" si="0">1/27</f>
@@ -685,16 +682,16 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -702,7 +699,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
@@ -724,16 +721,16 @@
         <v>1.25</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -741,7 +738,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
@@ -762,16 +759,16 @@
         <v>0.75</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -779,7 +776,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
@@ -799,16 +796,16 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -816,7 +813,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
@@ -837,16 +834,16 @@
         <v>1.25</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -854,7 +851,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
@@ -876,16 +873,16 @@
         <v>0.75</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -893,7 +890,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
@@ -914,16 +911,16 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -931,7 +928,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
@@ -953,16 +950,16 @@
         <v>1.25</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -970,7 +967,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
@@ -991,16 +988,16 @@
         <v>0.75</v>
       </c>
       <c r="H11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1008,7 +1005,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
@@ -1028,16 +1025,16 @@
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1045,7 +1042,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
@@ -1066,16 +1063,16 @@
         <v>1.25</v>
       </c>
       <c r="H13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1083,7 +1080,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
@@ -1103,16 +1100,16 @@
         <v>0.75</v>
       </c>
       <c r="H14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1120,7 +1117,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
@@ -1139,16 +1136,16 @@
         <v>1</v>
       </c>
       <c r="H15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1156,7 +1153,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
@@ -1176,16 +1173,16 @@
         <v>1.25</v>
       </c>
       <c r="H16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1193,7 +1190,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
@@ -1214,16 +1211,16 @@
         <v>0.75</v>
       </c>
       <c r="H17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -1231,7 +1228,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
@@ -1251,16 +1248,16 @@
         <v>1</v>
       </c>
       <c r="H18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -1268,7 +1265,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
@@ -1289,16 +1286,16 @@
         <v>1.25</v>
       </c>
       <c r="H19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -1306,7 +1303,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
@@ -1328,16 +1325,16 @@
         <v>0.75</v>
       </c>
       <c r="H20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -1345,7 +1342,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
@@ -1366,16 +1363,16 @@
         <v>1</v>
       </c>
       <c r="H21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1383,7 +1380,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
@@ -1405,16 +1402,16 @@
         <v>1.25</v>
       </c>
       <c r="H22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1422,7 +1419,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
@@ -1443,16 +1440,16 @@
         <v>0.75</v>
       </c>
       <c r="H23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1460,7 +1457,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
@@ -1480,16 +1477,16 @@
         <v>1</v>
       </c>
       <c r="H24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1497,7 +1494,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
@@ -1518,16 +1515,16 @@
         <v>1.25</v>
       </c>
       <c r="H25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -1535,7 +1532,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
@@ -1557,16 +1554,16 @@
         <v>0.75</v>
       </c>
       <c r="H26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -1574,7 +1571,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
@@ -1595,16 +1592,16 @@
         <v>1</v>
       </c>
       <c r="H27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -1612,7 +1609,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
@@ -1634,16 +1631,16 @@
         <v>1.25</v>
       </c>
       <c r="H28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1656,45 +1653,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D8424FF-558A-4FF4-BD92-4595B5988325}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1702,7 +1709,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2">
         <f>1/9</f>
@@ -1721,16 +1728,16 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -1738,7 +1745,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C10" si="0">1/9</f>
@@ -1760,16 +1767,16 @@
         <v>0.75</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1777,7 +1784,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
@@ -1799,16 +1806,16 @@
         <v>1.25</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -1816,7 +1823,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
@@ -1838,16 +1845,16 @@
         <v>0.75</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -1855,7 +1862,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
@@ -1877,16 +1884,16 @@
         <v>1.25</v>
       </c>
       <c r="H6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1894,7 +1901,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
@@ -1916,16 +1923,16 @@
         <v>0.75</v>
       </c>
       <c r="H7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1933,7 +1940,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
@@ -1955,16 +1962,16 @@
         <v>1.25</v>
       </c>
       <c r="H8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -1972,7 +1979,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
@@ -1994,16 +2001,16 @@
         <v>0.75</v>
       </c>
       <c r="H9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2011,7 +2018,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
@@ -2033,16 +2040,16 @@
         <v>1.25</v>
       </c>
       <c r="H10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2077,34 +2084,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2112,7 +2119,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <f>1/3</f>
@@ -2134,16 +2141,16 @@
         <v>0.75</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -2151,7 +2158,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3">
         <f>1/3</f>
@@ -2170,16 +2177,16 @@
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2187,7 +2194,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4">
         <f>1/3</f>
@@ -2209,16 +2216,16 @@
         <v>1.25</v>
       </c>
       <c r="H4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2255,34 +2262,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -2290,7 +2297,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2">
         <f>1/4</f>
@@ -2312,16 +2319,16 @@
         <v>0.75</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2329,7 +2336,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3">
         <f>1/4</f>
@@ -2351,16 +2358,16 @@
         <v>0.75</v>
       </c>
       <c r="H3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -2368,7 +2375,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4">
         <f>1/4</f>
@@ -2390,16 +2397,16 @@
         <v>1.25</v>
       </c>
       <c r="H4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2407,7 +2414,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5">
         <f>1/4</f>
@@ -2426,19 +2433,19 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2462,34 +2469,34 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -2497,7 +2504,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2515,16 +2522,16 @@
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2545,7 +2552,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -2563,8 +2570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAD9A92-DA97-41D6-8F28-B69416D7D7DA}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2624,9 +2631,6 @@
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2635,9 +2639,6 @@
       <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2701,9 +2702,6 @@
       <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -2712,9 +2710,6 @@
       <c r="B13" t="s">
         <v>9</v>
       </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -2774,12 +2769,6 @@
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>16</v>
-      </c>
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>